<commit_message>
Forced cell data type to String when no mapping is specified.
</commit_message>
<xml_diff>
--- a/src/test/resources/spreadsheets/generic.xlsx
+++ b/src/test/resources/spreadsheets/generic.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="13">
   <si>
     <t>First Name</t>
   </si>
@@ -63,13 +63,16 @@
   </si>
   <si>
     <t>looks||like||a||list</t>
+  </si>
+  <si>
+    <t>Extra Number</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -81,6 +84,22 @@
       <b/>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -103,14 +122,26 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="7">
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -386,25 +417,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F4"/>
+  <dimension ref="A1:G4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
@@ -423,8 +454,11 @@
       <c r="F3" s="1" t="s">
         <v>10</v>
       </c>
+      <c r="G3" s="1" t="s">
+        <v>12</v>
+      </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -442,9 +476,13 @@
       </c>
       <c r="F4" t="s">
         <v>11</v>
+      </c>
+      <c r="G4">
+        <v>123</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Defined integration test for modular spreadsheet mapping.
</commit_message>
<xml_diff>
--- a/src/test/resources/spreadsheets/generic.xlsx
+++ b/src/test/resources/spreadsheets/generic.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="54400" yWindow="3840" windowWidth="25600" windowHeight="14160" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Profile" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="18">
   <si>
     <t>First Name</t>
   </si>
@@ -66,6 +66,21 @@
   </si>
   <si>
     <t>Extra Number</t>
+  </si>
+  <si>
+    <t>Favorite Languages</t>
+  </si>
+  <si>
+    <t>Java||Python</t>
+  </si>
+  <si>
+    <t>Years of Experience</t>
+  </si>
+  <si>
+    <t>Developer Grade</t>
+  </si>
+  <si>
+    <t>Senior</t>
   </si>
 </sst>
 </file>
@@ -417,25 +432,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G4"/>
+  <dimension ref="A1:J4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+      <selection activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
@@ -457,8 +472,17 @@
       <c r="G3" s="1" t="s">
         <v>12</v>
       </c>
+      <c r="H3" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="J3" s="1" t="s">
+        <v>15</v>
+      </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -479,6 +503,15 @@
       </c>
       <c r="G4">
         <v>123</v>
+      </c>
+      <c r="H4" t="s">
+        <v>17</v>
+      </c>
+      <c r="I4" t="s">
+        <v>14</v>
+      </c>
+      <c r="J4">
+        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated importer code to process multiple records.
</commit_message>
<xml_diff>
--- a/src/test/resources/spreadsheets/generic.xlsx
+++ b/src/test/resources/spreadsheets/generic.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="29">
   <si>
     <t>First Name</t>
   </si>
@@ -81,6 +81,39 @@
   </si>
   <si>
     <t>Senior</t>
+  </si>
+  <si>
+    <t>Junior</t>
+  </si>
+  <si>
+    <t>John</t>
+  </si>
+  <si>
+    <t>Doe</t>
+  </si>
+  <si>
+    <t>Python</t>
+  </si>
+  <si>
+    <t>Jessica||Kaz||David</t>
+  </si>
+  <si>
+    <t>Mary</t>
+  </si>
+  <si>
+    <t>Moon</t>
+  </si>
+  <si>
+    <t>Vegetables</t>
+  </si>
+  <si>
+    <t>She's a vegetarian</t>
+  </si>
+  <si>
+    <t>Haskell||Perl||Erlang</t>
+  </si>
+  <si>
+    <t>Mid</t>
   </si>
 </sst>
 </file>
@@ -432,10 +465,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J4"/>
+  <dimension ref="A1:J6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H5" sqref="H5"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -514,6 +547,55 @@
         <v>20</v>
       </c>
     </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>19</v>
+      </c>
+      <c r="B5" t="s">
+        <v>20</v>
+      </c>
+      <c r="C5">
+        <v>23</v>
+      </c>
+      <c r="D5" t="s">
+        <v>22</v>
+      </c>
+      <c r="H5" t="s">
+        <v>18</v>
+      </c>
+      <c r="I5" t="s">
+        <v>21</v>
+      </c>
+      <c r="J5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>23</v>
+      </c>
+      <c r="B6" t="s">
+        <v>24</v>
+      </c>
+      <c r="C6">
+        <v>25</v>
+      </c>
+      <c r="D6" t="s">
+        <v>25</v>
+      </c>
+      <c r="E6" t="s">
+        <v>26</v>
+      </c>
+      <c r="H6" t="s">
+        <v>28</v>
+      </c>
+      <c r="I6" t="s">
+        <v>27</v>
+      </c>
+      <c r="J6">
+        <v>5</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>

<commit_message>
Updated WorksheetImporter to support custom array name.
</commit_message>
<xml_diff>
--- a/src/test/resources/spreadsheets/generic.xlsx
+++ b/src/test/resources/spreadsheets/generic.xlsx
@@ -9,10 +9,11 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" tabRatio="500"/>
+    <workbookView xWindow="54400" yWindow="3840" windowWidth="25600" windowHeight="14160" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Profile" sheetId="1" r:id="rId1"/>
+    <sheet name="Product" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="150000" concurrentCalc="0"/>
   <extLst>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="39">
   <si>
     <t>First Name</t>
   </si>
@@ -114,13 +115,43 @@
   </si>
   <si>
     <t>Mid</t>
+  </si>
+  <si>
+    <t>ID</t>
+  </si>
+  <si>
+    <t>NAME</t>
+  </si>
+  <si>
+    <t>QUANTITY</t>
+  </si>
+  <si>
+    <t>A001</t>
+  </si>
+  <si>
+    <t>Cheese</t>
+  </si>
+  <si>
+    <t>A002</t>
+  </si>
+  <si>
+    <t>Butter</t>
+  </si>
+  <si>
+    <t>A003</t>
+  </si>
+  <si>
+    <t>Milk</t>
+  </si>
+  <si>
+    <t>Reserved row</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -152,6 +183,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <i/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -179,9 +218,10 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="7">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -467,7 +507,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
@@ -600,4 +640,73 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1" s="2" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2" s="2" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>32</v>
+      </c>
+      <c r="B4" t="s">
+        <v>33</v>
+      </c>
+      <c r="C4">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>34</v>
+      </c>
+      <c r="B5" t="s">
+        <v>35</v>
+      </c>
+      <c r="C5">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>36</v>
+      </c>
+      <c r="B6" t="s">
+        <v>37</v>
+      </c>
+      <c r="C6">
+        <v>37</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Added check for empty rows.
</commit_message>
<xml_diff>
--- a/src/test/resources/spreadsheets/generic.xlsx
+++ b/src/test/resources/spreadsheets/generic.xlsx
@@ -9,11 +9,12 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="54400" yWindow="3840" windowWidth="25600" windowHeight="14160" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="54400" yWindow="3840" windowWidth="25600" windowHeight="14160" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Profile" sheetId="1" r:id="rId1"/>
     <sheet name="Product" sheetId="2" r:id="rId2"/>
+    <sheet name="Expenses" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="150000" concurrentCalc="0"/>
   <extLst>
@@ -28,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="46">
   <si>
     <t>First Name</t>
   </si>
@@ -126,6 +127,9 @@
     <t>QUANTITY</t>
   </si>
   <si>
+    <t>A1</t>
+  </si>
+  <si>
     <t>A001</t>
   </si>
   <si>
@@ -145,6 +149,24 @@
   </si>
   <si>
     <t>Reserved row</t>
+  </si>
+  <si>
+    <t>Amount</t>
+  </si>
+  <si>
+    <t>Entry No</t>
+  </si>
+  <si>
+    <t>A2</t>
+  </si>
+  <si>
+    <t>A3</t>
+  </si>
+  <si>
+    <t>A4</t>
+  </si>
+  <si>
+    <t>A6</t>
   </si>
 </sst>
 </file>
@@ -218,10 +240,12 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="7">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -505,10 +529,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J6"/>
+  <dimension ref="A1:J7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -635,6 +659,9 @@
       <c r="J6">
         <v>5</v>
       </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A7" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -646,7 +673,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
@@ -654,12 +681,12 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
@@ -675,10 +702,10 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B4" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C4">
         <v>24</v>
@@ -686,10 +713,10 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B5" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C5">
         <v>17</v>
@@ -697,13 +724,86 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B6" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C6">
         <v>37</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B9"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A10" sqref="A10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1" s="2" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2" s="2" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="B4">
+        <v>3.09</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="B5">
+        <v>2.5499999999999998</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A6" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="B6">
+        <v>10.77</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A7" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="B7">
+        <v>5.6</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A9" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="B9">
+        <v>2.56</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated test spreadsheet to fix integration tests.
</commit_message>
<xml_diff>
--- a/src/test/resources/spreadsheets/generic.xlsx
+++ b/src/test/resources/spreadsheets/generic.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="54400" yWindow="3840" windowWidth="25600" windowHeight="14160" tabRatio="500" activeTab="2"/>
+    <workbookView xWindow="54400" yWindow="3840" windowWidth="25600" windowHeight="14160" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Profile" sheetId="1" r:id="rId1"/>
@@ -240,11 +240,10 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="7">
@@ -529,10 +528,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J7"/>
+  <dimension ref="A1:J6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -659,9 +658,6 @@
       <c r="J6">
         <v>5</v>
       </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A7" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -742,8 +738,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -767,7 +763,7 @@
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A4" s="4" t="s">
+      <c r="A4" s="3" t="s">
         <v>32</v>
       </c>
       <c r="B4">
@@ -775,7 +771,7 @@
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A5" s="4" t="s">
+      <c r="A5" s="3" t="s">
         <v>42</v>
       </c>
       <c r="B5">
@@ -783,7 +779,7 @@
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A6" s="4" t="s">
+      <c r="A6" s="3" t="s">
         <v>43</v>
       </c>
       <c r="B6">
@@ -791,7 +787,7 @@
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A7" s="4" t="s">
+      <c r="A7" s="3" t="s">
         <v>44</v>
       </c>
       <c r="B7">
@@ -799,7 +795,7 @@
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A9" s="4" t="s">
+      <c r="A9" s="3" t="s">
         <v>45</v>
       </c>
       <c r="B9">

</xml_diff>